<commit_message>
calculated average and median differences amongst parties
</commit_message>
<xml_diff>
--- a/data/predictions/diffs/DvI.xlsx
+++ b/data/predictions/diffs/DvI.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="196">
   <si>
     <t>abortion Predicted unrestricted</t>
   </si>
@@ -596,6 +596,12 @@
   </si>
   <si>
     <t>spending/alt_energy Too little</t>
+  </si>
+  <si>
+    <t>median</t>
+  </si>
+  <si>
+    <t>mean</t>
   </si>
 </sst>
 </file>
@@ -953,13 +959,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:GM39"/>
+  <dimension ref="A1:GO39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:195">
+    <row r="1" spans="1:197">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1542,8 +1548,14 @@
       <c r="GM1" s="1" t="s">
         <v>193</v>
       </c>
+      <c r="GN1" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="GO1" s="1" t="s">
+        <v>195</v>
+      </c>
     </row>
-    <row r="2" spans="1:195">
+    <row r="2" spans="1:197">
       <c r="A2" s="1">
         <v>1972</v>
       </c>
@@ -1565,8 +1577,14 @@
       <c r="Q2">
         <v>0.03932837609103515</v>
       </c>
+      <c r="GN2">
+        <v>0.03285440856456028</v>
+      </c>
+      <c r="GO2">
+        <v>0.02853783047579867</v>
+      </c>
     </row>
-    <row r="3" spans="1:195">
+    <row r="3" spans="1:197">
       <c r="A3" s="1">
         <v>1973</v>
       </c>
@@ -1693,8 +1711,14 @@
       <c r="GG3">
         <v>0.08869981587619402</v>
       </c>
+      <c r="GN3">
+        <v>0.02755272203484037</v>
+      </c>
+      <c r="GO3">
+        <v>0.0401034855044566</v>
+      </c>
     </row>
-    <row r="4" spans="1:195">
+    <row r="4" spans="1:197">
       <c r="A4" s="1">
         <v>1974</v>
       </c>
@@ -1830,8 +1854,14 @@
       <c r="GG4">
         <v>0.04575614728024846</v>
       </c>
+      <c r="GN4">
+        <v>0.01965076489533008</v>
+      </c>
+      <c r="GO4">
+        <v>0.02418650682259138</v>
+      </c>
     </row>
-    <row r="5" spans="1:195">
+    <row r="5" spans="1:197">
       <c r="A5" s="1">
         <v>1975</v>
       </c>
@@ -1988,8 +2018,14 @@
       <c r="GG5">
         <v>0.01946329728063467</v>
       </c>
+      <c r="GN5">
+        <v>0.03408115413539169</v>
+      </c>
+      <c r="GO5">
+        <v>0.04216732468472677</v>
+      </c>
     </row>
-    <row r="6" spans="1:195">
+    <row r="6" spans="1:197">
       <c r="A6" s="1">
         <v>1976</v>
       </c>
@@ -2131,8 +2167,14 @@
       <c r="GG6">
         <v>0.01794896765539067</v>
       </c>
+      <c r="GN6">
+        <v>0.02785415740270621</v>
+      </c>
+      <c r="GO6">
+        <v>0.03314734242471936</v>
+      </c>
     </row>
-    <row r="7" spans="1:195">
+    <row r="7" spans="1:197">
       <c r="A7" s="1">
         <v>1977</v>
       </c>
@@ -2292,8 +2334,14 @@
       <c r="GG7">
         <v>0.03568242145128631</v>
       </c>
+      <c r="GN7">
+        <v>0.01937860433113033</v>
+      </c>
+      <c r="GO7">
+        <v>0.03066725527911303</v>
+      </c>
     </row>
-    <row r="8" spans="1:195">
+    <row r="8" spans="1:197">
       <c r="A8" s="1">
         <v>1978</v>
       </c>
@@ -2435,8 +2483,14 @@
       <c r="GG8">
         <v>0.002839074437363642</v>
       </c>
+      <c r="GN8">
+        <v>0.0254277931161527</v>
+      </c>
+      <c r="GO8">
+        <v>0.03277633436352156</v>
+      </c>
     </row>
-    <row r="9" spans="1:195">
+    <row r="9" spans="1:197">
       <c r="A9" s="1">
         <v>1980</v>
       </c>
@@ -2569,8 +2623,14 @@
       <c r="GG9">
         <v>0.03587833645135186</v>
       </c>
+      <c r="GN9">
+        <v>0.03633143445512643</v>
+      </c>
+      <c r="GO9">
+        <v>0.03828066581938715</v>
+      </c>
     </row>
-    <row r="10" spans="1:195">
+    <row r="10" spans="1:197">
       <c r="A10" s="1">
         <v>1982</v>
       </c>
@@ -2706,8 +2766,14 @@
       <c r="GG10">
         <v>0.09715689728060473</v>
       </c>
+      <c r="GN10">
+        <v>0.04532672586015944</v>
+      </c>
+      <c r="GO10">
+        <v>0.05264547661864068</v>
+      </c>
     </row>
-    <row r="11" spans="1:195">
+    <row r="11" spans="1:197">
       <c r="A11" s="1">
         <v>1983</v>
       </c>
@@ -2864,8 +2930,14 @@
       <c r="GG11">
         <v>0.07940935192780962</v>
       </c>
+      <c r="GN11">
+        <v>0.03274086227326588</v>
+      </c>
+      <c r="GO11">
+        <v>0.03815921276152804</v>
+      </c>
     </row>
-    <row r="12" spans="1:195">
+    <row r="12" spans="1:197">
       <c r="A12" s="1">
         <v>1984</v>
       </c>
@@ -3049,8 +3121,14 @@
       <c r="GG12">
         <v>0.006554494583910775</v>
       </c>
+      <c r="GN12">
+        <v>0.04267665892590883</v>
+      </c>
+      <c r="GO12">
+        <v>0.04734141505915695</v>
+      </c>
     </row>
-    <row r="13" spans="1:195">
+    <row r="13" spans="1:197">
       <c r="A13" s="1">
         <v>1985</v>
       </c>
@@ -3246,8 +3324,14 @@
       <c r="GG13">
         <v>0.1306915807560138</v>
       </c>
+      <c r="GN13">
+        <v>0.04349757932343196</v>
+      </c>
+      <c r="GO13">
+        <v>0.04546515254080564</v>
+      </c>
     </row>
-    <row r="14" spans="1:195">
+    <row r="14" spans="1:197">
       <c r="A14" s="1">
         <v>1986</v>
       </c>
@@ -3455,8 +3539,14 @@
       <c r="GG14">
         <v>0.05265346431727225</v>
       </c>
+      <c r="GN14">
+        <v>0.0393070092860975</v>
+      </c>
+      <c r="GO14">
+        <v>0.05201809402526514</v>
+      </c>
     </row>
-    <row r="15" spans="1:195">
+    <row r="15" spans="1:197">
       <c r="A15" s="1">
         <v>1987</v>
       </c>
@@ -3640,8 +3730,14 @@
       <c r="GG15">
         <v>0.08470853330731076</v>
       </c>
+      <c r="GN15">
+        <v>0.03067360192769471</v>
+      </c>
+      <c r="GO15">
+        <v>0.0469421887066003</v>
+      </c>
     </row>
-    <row r="16" spans="1:195">
+    <row r="16" spans="1:197">
       <c r="A16" s="1">
         <v>1988</v>
       </c>
@@ -3873,8 +3969,14 @@
       <c r="GG16">
         <v>0.009392326358655834</v>
       </c>
+      <c r="GN16">
+        <v>0.02536763926865549</v>
+      </c>
+      <c r="GO16">
+        <v>0.038955425437353</v>
+      </c>
     </row>
-    <row r="17" spans="1:195">
+    <row r="17" spans="1:197">
       <c r="A17" s="1">
         <v>1989</v>
       </c>
@@ -4091,8 +4193,14 @@
       <c r="GG17">
         <v>0.03881485737217905</v>
       </c>
+      <c r="GN17">
+        <v>0.03662211388404191</v>
+      </c>
+      <c r="GO17">
+        <v>0.04133935008587139</v>
+      </c>
     </row>
-    <row r="18" spans="1:195">
+    <row r="18" spans="1:197">
       <c r="A18" s="1">
         <v>1990</v>
       </c>
@@ -4318,8 +4426,14 @@
       <c r="GG18">
         <v>0.07907342116330185</v>
       </c>
+      <c r="GN18">
+        <v>0.04098778455393001</v>
+      </c>
+      <c r="GO18">
+        <v>0.042771459998787</v>
+      </c>
     </row>
-    <row r="19" spans="1:195">
+    <row r="19" spans="1:197">
       <c r="A19" s="1">
         <v>1991</v>
       </c>
@@ -4536,8 +4650,14 @@
       <c r="GG19">
         <v>0.06683784694909534</v>
       </c>
+      <c r="GN19">
+        <v>0.04796064267122746</v>
+      </c>
+      <c r="GO19">
+        <v>0.04862403392917938</v>
+      </c>
     </row>
-    <row r="20" spans="1:195">
+    <row r="20" spans="1:197">
       <c r="A20" s="1">
         <v>1993</v>
       </c>
@@ -4754,8 +4874,14 @@
       <c r="GG20">
         <v>0.08456756247320663</v>
       </c>
+      <c r="GN20">
+        <v>0.0283096857746935</v>
+      </c>
+      <c r="GO20">
+        <v>0.04004979720575044</v>
+      </c>
     </row>
-    <row r="21" spans="1:195">
+    <row r="21" spans="1:197">
       <c r="A21" s="1">
         <v>1994</v>
       </c>
@@ -4993,8 +5119,14 @@
       <c r="GG21">
         <v>0.08605907899090204</v>
       </c>
+      <c r="GN21">
+        <v>0.04479098901783383</v>
+      </c>
+      <c r="GO21">
+        <v>0.0553213337299854</v>
+      </c>
     </row>
-    <row r="22" spans="1:195">
+    <row r="22" spans="1:197">
       <c r="A22" s="1">
         <v>1996</v>
       </c>
@@ -5232,8 +5364,14 @@
       <c r="GG22">
         <v>0.05096109180499453</v>
       </c>
+      <c r="GN22">
+        <v>0.0345048704127461</v>
+      </c>
+      <c r="GO22">
+        <v>0.04138113423598297</v>
+      </c>
     </row>
-    <row r="23" spans="1:195">
+    <row r="23" spans="1:197">
       <c r="A23" s="1">
         <v>1998</v>
       </c>
@@ -5471,8 +5609,14 @@
       <c r="GG23">
         <v>0.05667623238403352</v>
       </c>
+      <c r="GN23">
+        <v>0.04328053978814657</v>
+      </c>
+      <c r="GO23">
+        <v>0.04713347507228979</v>
+      </c>
     </row>
-    <row r="24" spans="1:195">
+    <row r="24" spans="1:197">
       <c r="A24" s="1">
         <v>2000</v>
       </c>
@@ -5719,8 +5863,14 @@
       <c r="GG24">
         <v>0.1391125550262416</v>
       </c>
+      <c r="GN24">
+        <v>0.03101679295986759</v>
+      </c>
+      <c r="GO24">
+        <v>0.0419735020549061</v>
+      </c>
     </row>
-    <row r="25" spans="1:195">
+    <row r="25" spans="1:197">
       <c r="A25" s="1">
         <v>2002</v>
       </c>
@@ -5976,8 +6126,14 @@
       <c r="GG25">
         <v>0.0718385254844135</v>
       </c>
+      <c r="GN25">
+        <v>0.02983280177363729</v>
+      </c>
+      <c r="GO25">
+        <v>0.03871561571854708</v>
+      </c>
     </row>
-    <row r="26" spans="1:195">
+    <row r="26" spans="1:197">
       <c r="A26" s="1">
         <v>2004</v>
       </c>
@@ -6263,8 +6419,14 @@
       <c r="GG26">
         <v>0.02829610255922654</v>
       </c>
+      <c r="GN26">
+        <v>0.04155238736148028</v>
+      </c>
+      <c r="GO26">
+        <v>0.05207445293199564</v>
+      </c>
     </row>
-    <row r="27" spans="1:195">
+    <row r="27" spans="1:197">
       <c r="A27" s="1">
         <v>2006</v>
       </c>
@@ -6550,8 +6712,14 @@
       <c r="GG27">
         <v>0.09644455248539197</v>
       </c>
+      <c r="GN27">
+        <v>0.03794947492770474</v>
+      </c>
+      <c r="GO27">
+        <v>0.04771070083594445</v>
+      </c>
     </row>
-    <row r="28" spans="1:195">
+    <row r="28" spans="1:197">
       <c r="A28" s="1">
         <v>2008</v>
       </c>
@@ -6837,8 +7005,14 @@
       <c r="GG28">
         <v>0.06287247912405181</v>
       </c>
+      <c r="GN28">
+        <v>0.04176630428601012</v>
+      </c>
+      <c r="GO28">
+        <v>0.05220129192850576</v>
+      </c>
     </row>
-    <row r="29" spans="1:195">
+    <row r="29" spans="1:197">
       <c r="A29" s="1">
         <v>2010</v>
       </c>
@@ -7133,8 +7307,14 @@
       <c r="GM29">
         <v>0.05489425583405405</v>
       </c>
+      <c r="GN29">
+        <v>0.04396626545484317</v>
+      </c>
+      <c r="GO29">
+        <v>0.05529598297025578</v>
+      </c>
     </row>
-    <row r="30" spans="1:195">
+    <row r="30" spans="1:197">
       <c r="A30" s="1">
         <v>2012</v>
       </c>
@@ -7429,8 +7609,14 @@
       <c r="GM30">
         <v>0.05767991785895521</v>
       </c>
+      <c r="GN30">
+        <v>0.05947401499433308</v>
+      </c>
+      <c r="GO30">
+        <v>0.06047632659264623</v>
+      </c>
     </row>
-    <row r="31" spans="1:195">
+    <row r="31" spans="1:197">
       <c r="A31" s="1">
         <v>2014</v>
       </c>
@@ -7725,8 +7911,14 @@
       <c r="GM31">
         <v>0.08367400338564557</v>
       </c>
+      <c r="GN31">
+        <v>0.05173806730446739</v>
+      </c>
+      <c r="GO31">
+        <v>0.05798589891502316</v>
+      </c>
     </row>
-    <row r="32" spans="1:195">
+    <row r="32" spans="1:197">
       <c r="A32" s="1">
         <v>2016</v>
       </c>
@@ -8021,8 +8213,14 @@
       <c r="GM32">
         <v>0.08406892144771616</v>
       </c>
+      <c r="GN32">
+        <v>0.04785520980266225</v>
+      </c>
+      <c r="GO32">
+        <v>0.06068782307594302</v>
+      </c>
     </row>
-    <row r="33" spans="1:195">
+    <row r="33" spans="1:197">
       <c r="A33" s="1">
         <v>2018</v>
       </c>
@@ -8317,8 +8515,14 @@
       <c r="GM33">
         <v>0.07126191723847664</v>
       </c>
+      <c r="GN33">
+        <v>0.05979293514149104</v>
+      </c>
+      <c r="GO33">
+        <v>0.07234216568031356</v>
+      </c>
     </row>
-    <row r="34" spans="1:195">
+    <row r="34" spans="1:197">
       <c r="A34" s="1">
         <v>2019</v>
       </c>
@@ -8613,8 +8817,14 @@
       <c r="GL34">
         <v>0.07031580277258753</v>
       </c>
+      <c r="GN34">
+        <v>0.069765323146046</v>
+      </c>
+      <c r="GO34">
+        <v>0.08131974350379645</v>
+      </c>
     </row>
-    <row r="35" spans="1:195">
+    <row r="35" spans="1:197">
       <c r="A35" s="1">
         <v>2020</v>
       </c>
@@ -8909,8 +9119,14 @@
       <c r="GL35">
         <v>0.07031580277258753</v>
       </c>
+      <c r="GN35">
+        <v>0.06883674994238953</v>
+      </c>
+      <c r="GO35">
+        <v>0.08745639917045274</v>
+      </c>
     </row>
-    <row r="36" spans="1:195">
+    <row r="36" spans="1:197">
       <c r="A36" s="1">
         <v>2021</v>
       </c>
@@ -9205,8 +9421,14 @@
       <c r="GL36">
         <v>0.07031580277258753</v>
       </c>
+      <c r="GN36">
+        <v>0.07678965979778807</v>
+      </c>
+      <c r="GO36">
+        <v>0.09467446729125548</v>
+      </c>
     </row>
-    <row r="37" spans="1:195">
+    <row r="37" spans="1:197">
       <c r="A37" s="1">
         <v>2022</v>
       </c>
@@ -9501,8 +9723,14 @@
       <c r="GL37">
         <v>0.07031580277258753</v>
       </c>
+      <c r="GN37">
+        <v>0.0702439680357677</v>
+      </c>
+      <c r="GO37">
+        <v>0.09974756583769276</v>
+      </c>
     </row>
-    <row r="38" spans="1:195">
+    <row r="38" spans="1:197">
       <c r="A38" s="1">
         <v>2023</v>
       </c>
@@ -9797,8 +10025,14 @@
       <c r="GL38">
         <v>0.07031580277258753</v>
       </c>
+      <c r="GN38">
+        <v>0.07031580277258753</v>
+      </c>
+      <c r="GO38">
+        <v>0.1026572806889232</v>
+      </c>
     </row>
-    <row r="39" spans="1:195">
+    <row r="39" spans="1:197">
       <c r="A39" s="1">
         <v>2024</v>
       </c>
@@ -10092,6 +10326,12 @@
       </c>
       <c r="GL39">
         <v>0.07031580277258753</v>
+      </c>
+      <c r="GN39">
+        <v>0.07203577175959819</v>
+      </c>
+      <c r="GO39">
+        <v>0.1089851809530814</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added median to calculations
</commit_message>
<xml_diff>
--- a/data/predictions/diffs/DvI.xlsx
+++ b/data/predictions/diffs/DvI.xlsx
@@ -1578,10 +1578,10 @@
         <v>0.03932837609103515</v>
       </c>
       <c r="GN2">
-        <v>0.03285440856456028</v>
+        <v>0.03134702070097369</v>
       </c>
       <c r="GO2">
-        <v>0.02853783047579867</v>
+        <v>0.02829837563288518</v>
       </c>
     </row>
     <row r="3" spans="1:197">
@@ -1855,10 +1855,10 @@
         <v>0.04575614728024846</v>
       </c>
       <c r="GN4">
-        <v>0.01965076489533008</v>
+        <v>0.01974571783222141</v>
       </c>
       <c r="GO4">
-        <v>0.02418650682259138</v>
+        <v>0.02418866206513855</v>
       </c>
     </row>
     <row r="5" spans="1:197">
@@ -2168,10 +2168,10 @@
         <v>0.01794896765539067</v>
       </c>
       <c r="GN6">
-        <v>0.02785415740270621</v>
+        <v>0.02814017066518326</v>
       </c>
       <c r="GO6">
-        <v>0.03314734242471936</v>
+        <v>0.03315355275802522</v>
       </c>
     </row>
     <row r="7" spans="1:197">
@@ -2335,10 +2335,10 @@
         <v>0.03568242145128631</v>
       </c>
       <c r="GN7">
-        <v>0.01937860433113033</v>
+        <v>0.01952052143092185</v>
       </c>
       <c r="GO7">
-        <v>0.03066725527911303</v>
+        <v>0.03066998191207402</v>
       </c>
     </row>
     <row r="8" spans="1:197">
@@ -2484,10 +2484,10 @@
         <v>0.002839074437363642</v>
       </c>
       <c r="GN8">
-        <v>0.0254277931161527</v>
+        <v>0.02588784202292533</v>
       </c>
       <c r="GO8">
-        <v>0.03277633436352156</v>
+        <v>0.03278632361025548</v>
       </c>
     </row>
     <row r="9" spans="1:197">
@@ -2767,10 +2767,10 @@
         <v>0.09715689728060473</v>
       </c>
       <c r="GN10">
-        <v>0.04532672586015944</v>
+        <v>0.04690698430016065</v>
       </c>
       <c r="GO10">
-        <v>0.05264547661864068</v>
+        <v>0.05268134533778649</v>
       </c>
     </row>
     <row r="11" spans="1:197">
@@ -3122,10 +3122,10 @@
         <v>0.006554494583910775</v>
       </c>
       <c r="GN12">
-        <v>0.04267665892590883</v>
+        <v>0.04311953570400399</v>
       </c>
       <c r="GO12">
-        <v>0.04734141505915695</v>
+        <v>0.04734879113564756</v>
       </c>
     </row>
     <row r="13" spans="1:197">
@@ -3325,10 +3325,10 @@
         <v>0.1306915807560138</v>
       </c>
       <c r="GN13">
-        <v>0.04349757932343196</v>
+        <v>0.04355853372891137</v>
       </c>
       <c r="GO13">
-        <v>0.04546515254080564</v>
+        <v>0.0454661043615069</v>
       </c>
     </row>
     <row r="14" spans="1:197">
@@ -3540,10 +3540,10 @@
         <v>0.05265346431727225</v>
       </c>
       <c r="GN14">
-        <v>0.0393070092860975</v>
+        <v>0.03998567698783914</v>
       </c>
       <c r="GO14">
-        <v>0.05201809402526514</v>
+        <v>0.05202806892353641</v>
       </c>
     </row>
     <row r="15" spans="1:197">
@@ -3731,10 +3731,10 @@
         <v>0.08470853330731076</v>
       </c>
       <c r="GN15">
-        <v>0.03067360192769471</v>
+        <v>0.03109883439342404</v>
       </c>
       <c r="GO15">
-        <v>0.0469421887066003</v>
+        <v>0.04694927091851261</v>
       </c>
     </row>
     <row r="16" spans="1:197">
@@ -3970,10 +3970,10 @@
         <v>0.009392326358655834</v>
       </c>
       <c r="GN16">
-        <v>0.02536763926865549</v>
+        <v>0.02551708912600976</v>
       </c>
       <c r="GO16">
-        <v>0.038955425437353</v>
+        <v>0.03895739100988534</v>
       </c>
     </row>
     <row r="17" spans="1:197">
@@ -4427,10 +4427,10 @@
         <v>0.07907342116330185</v>
       </c>
       <c r="GN18">
-        <v>0.04098778455393001</v>
+        <v>0.04172867070894427</v>
       </c>
       <c r="GO18">
-        <v>0.042771459998787</v>
+        <v>0.04278146729070075</v>
       </c>
     </row>
     <row r="19" spans="1:197">
@@ -5120,10 +5120,10 @@
         <v>0.08605907899090204</v>
       </c>
       <c r="GN21">
-        <v>0.04479098901783383</v>
+        <v>0.04553391921489253</v>
       </c>
       <c r="GO21">
-        <v>0.0553213337299854</v>
+        <v>0.05533085445784926</v>
       </c>
     </row>
     <row r="22" spans="1:197">
@@ -5365,10 +5365,10 @@
         <v>0.05096109180499453</v>
       </c>
       <c r="GN22">
-        <v>0.0345048704127461</v>
+        <v>0.03473267791539486</v>
       </c>
       <c r="GO22">
-        <v>0.04138113423598297</v>
+        <v>0.04138405361285936</v>
       </c>
     </row>
     <row r="23" spans="1:197">
@@ -5610,10 +5610,10 @@
         <v>0.05667623238403352</v>
       </c>
       <c r="GN23">
-        <v>0.04328053978814657</v>
+        <v>0.04333266591548361</v>
       </c>
       <c r="GO23">
-        <v>0.04713347507228979</v>
+        <v>0.04713414307404142</v>
       </c>
     </row>
     <row r="24" spans="1:197">
@@ -6127,10 +6127,10 @@
         <v>0.0718385254844135</v>
       </c>
       <c r="GN25">
-        <v>0.02983280177363729</v>
+        <v>0.03008726834964569</v>
       </c>
       <c r="GO25">
-        <v>0.03871561571854708</v>
+        <v>0.03871864397759345</v>
       </c>
     </row>
     <row r="26" spans="1:197">
@@ -6420,10 +6420,10 @@
         <v>0.02829610255922654</v>
       </c>
       <c r="GN26">
-        <v>0.04155238736148028</v>
+        <v>0.04164763989158216</v>
       </c>
       <c r="GO26">
-        <v>0.05207445293199564</v>
+        <v>0.05207546596052232</v>
       </c>
     </row>
     <row r="27" spans="1:197">
@@ -6713,10 +6713,10 @@
         <v>0.09644455248539197</v>
       </c>
       <c r="GN27">
-        <v>0.03794947492770474</v>
+        <v>0.03806908299316895</v>
       </c>
       <c r="GO27">
-        <v>0.04771070083594445</v>
+        <v>0.04771197289015872</v>
       </c>
     </row>
     <row r="28" spans="1:197">
@@ -7006,10 +7006,10 @@
         <v>0.06287247912405181</v>
       </c>
       <c r="GN28">
-        <v>0.04176630428601012</v>
+        <v>0.04204889344109027</v>
       </c>
       <c r="GO28">
-        <v>0.05220129192850576</v>
+        <v>0.05220429731718276</v>
       </c>
     </row>
     <row r="29" spans="1:197">

</xml_diff>